<commit_message>
data driven done set parameters and grouping tests
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="6075" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="6075"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
     <sheet name="AccountCreationData" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:L18"/>
+  <oleSize ref="A4:E19"/>
 </workbook>
 </file>
 
@@ -201,9 +201,6 @@
     <t>M</t>
   </si>
   <si>
-    <t>ghfsdtyfg@gmail.com</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -298,6 +295,9 @@
   </si>
   <si>
     <t>ghjg@gmail.com</t>
+  </si>
+  <si>
+    <t>fdqff@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -767,8 +767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,7 +1027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1058,7 +1058,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="9">
         <v>123456</v>
@@ -1079,7 +1079,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1093,7 +1095,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>58</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1197,187 +1199,187 @@
         <v>52</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="F2" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="I2" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="F3" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" s="12" t="s">
+      <c r="J3" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="I3" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J3" s="12" t="s">
+      <c r="K3" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="L3" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="L3" s="12" t="s">
+      <c r="M3" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="M3" s="12" t="s">
+      <c r="N3" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="N3" s="12" t="s">
+      <c r="O3" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="12" t="s">
+      <c r="F4" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="H4" s="12" t="s">
+      <c r="J4" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="J4" s="12" t="s">
+      <c r="K4" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="L4" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="L4" s="12" t="s">
+      <c r="M4" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="N4" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="N4" s="12" t="s">
+      <c r="O4" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="O4" s="12" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>